<commit_message>
extract and parse schedule via Google sheets
Final upload I guess
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F35AA4-501E-4B04-93F3-1D2D2A0E0193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Группа</t>
   </si>
@@ -27,14 +28,62 @@
     <t>Ссылка на расписание</t>
   </si>
   <si>
+    <t>https://docs.google.com/spreadsheets/d/1E80xi4hgdd2JCox_hBIUjM08F5G6lRTfCC3E5K_7RoA/edit#gid=615601934</t>
+  </si>
+  <si>
     <t>20ФиПЛ-1</t>
+  </si>
+  <si>
+    <t>20ФиПЛ-2</t>
+  </si>
+  <si>
+    <t>20ФИЛ-1</t>
+  </si>
+  <si>
+    <t>20ФИЛ-2</t>
+  </si>
+  <si>
+    <t>23ФИЛ-1</t>
+  </si>
+  <si>
+    <t>23ФИЛ-2</t>
+  </si>
+  <si>
+    <t>23ФиПЛ-1</t>
+  </si>
+  <si>
+    <t>23ФиПЛ-2</t>
+  </si>
+  <si>
+    <t>22ФИЛ-1</t>
+  </si>
+  <si>
+    <t>22ФИЛ-2</t>
+  </si>
+  <si>
+    <t>22ФиПЛ-1</t>
+  </si>
+  <si>
+    <t>22ФиПЛ-2</t>
+  </si>
+  <si>
+    <t>21ФИЛ-1</t>
+  </si>
+  <si>
+    <t>21ФИЛ-2</t>
+  </si>
+  <si>
+    <t>21ФиПЛ-1</t>
+  </si>
+  <si>
+    <t>21ФиПЛ-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +98,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -69,10 +126,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -83,8 +141,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,11 +447,152 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="gid=615601934" xr:uid="{20DE9762-D468-4DE2-9927-14EC0F9315D3}"/>
+    <hyperlink ref="B3" r:id="rId2" location="gid=615601934" xr:uid="{37A72538-530C-4546-A9FD-E8A2FB28622E}"/>
+    <hyperlink ref="B4" r:id="rId3" location="gid=615601934" xr:uid="{CBCCAE00-6772-4639-8B99-651FA7565AE5}"/>
+    <hyperlink ref="B5" r:id="rId4" location="gid=615601934" xr:uid="{299D7741-D221-401B-B5F6-07E15E688F03}"/>
+    <hyperlink ref="B6" r:id="rId5" location="gid=615601934" xr:uid="{A0357B8E-844A-4BE4-B2F3-35E43DAC2E73}"/>
+    <hyperlink ref="B7" r:id="rId6" location="gid=615601934" xr:uid="{94900215-335C-4E4A-8ADB-2B86FD0BF1F9}"/>
+    <hyperlink ref="B8" r:id="rId7" location="gid=615601934" xr:uid="{0F7E3BD8-2E84-4EAD-BEFC-63ED72C47828}"/>
+    <hyperlink ref="B9" r:id="rId8" location="gid=615601934" xr:uid="{54EE85E0-60A8-49F3-B16E-746B9BB5F548}"/>
+    <hyperlink ref="B10" r:id="rId9" location="gid=615601934" xr:uid="{011FE6C6-C4F1-458D-B283-4BA4DCA4DDDE}"/>
+    <hyperlink ref="B11" r:id="rId10" location="gid=615601934" xr:uid="{BE421230-F367-4370-88F8-F5F9CF2B805C}"/>
+    <hyperlink ref="B12" r:id="rId11" location="gid=615601934" xr:uid="{5F0BEB1B-7361-404D-9705-5FFC62C42CD9}"/>
+    <hyperlink ref="B13" r:id="rId12" location="gid=615601934" xr:uid="{71D015CD-D070-4010-B628-3B2E82372E90}"/>
+    <hyperlink ref="B14" r:id="rId13" location="gid=615601934" xr:uid="{EB6AC9F4-6485-4EBB-87B1-62F0894EF476}"/>
+    <hyperlink ref="B15" r:id="rId14" location="gid=615601934" xr:uid="{DE54BD75-E4B6-4BED-B4E0-588E0E4E4D4B}"/>
+    <hyperlink ref="B16" r:id="rId15" location="gid=615601934" xr:uid="{6A95BA33-5DA3-4A16-BF0B-FBE532F82BA2}"/>
+    <hyperlink ref="B17" r:id="rId16" location="gid=615601934" xr:uid="{60DFFF1B-1435-4854-A066-F5C7699749FE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>